<commit_message>
10. gyak 1. feladat táblázat javítása
</commit_message>
<xml_diff>
--- a/AJYKQ3_04_22/AJYKQ3_10.gyak_1.xlsx
+++ b/AJYKQ3_04_22/AJYKQ3_10.gyak_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marty\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reporetekOS\AJYKQ3OsGyak\AJYKQ3_04_22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802B1072-72BD-4F2B-A313-BCDD46012176}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ACCAC0-A406-4326-BF9F-D6246EBA8A02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{4260EE31-A546-4710-86FB-97C7D8D8B52A}"/>
+    <workbookView xWindow="1728" yWindow="5160" windowWidth="23040" windowHeight="12660" xr2:uid="{4260EE31-A546-4710-86FB-97C7D8D8B52A}"/>
   </bookViews>
   <sheets>
     <sheet name="10.gyak 1. feladat AJYKQ3" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>Az összes erőforrások száma: (10,5,7)</t>
   </si>
@@ -141,7 +141,10 @@
     <t>Nem elégíthető ki egyik processz erőforrásigénye sem</t>
   </si>
   <si>
-    <t>Nem biztonságos a rendszer</t>
+    <t>Biztonságos a rendszer</t>
+  </si>
+  <si>
+    <t>Processzek futási sorrendje</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -217,6 +220,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -554,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D98912-E991-4B49-8F5B-FC64DC9A45E8}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,8 +570,9 @@
     <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1019,6 +1026,9 @@
       <c r="K26" t="s">
         <v>6</v>
       </c>
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1060,7 +1070,7 @@
       <c r="M27" t="s">
         <v>30</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1104,7 +1114,7 @@
       <c r="M28" t="s">
         <v>29</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1148,7 +1158,7 @@
       <c r="M29" t="s">
         <v>31</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1192,7 +1202,7 @@
       <c r="M30" t="s">
         <v>32</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1236,7 +1246,7 @@
       <c r="M31" t="s">
         <v>33</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="7">
         <v>5</v>
       </c>
     </row>

</xml_diff>